<commit_message>
Finished JS performance tests. Added section to chapter 4 about the JS performance tests.
</commit_message>
<xml_diff>
--- a/Test data.xlsx
+++ b/Test data.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11540" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="JS performance" sheetId="1" r:id="rId1"/>
+    <sheet name="Server side response time" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Browser</t>
-  </si>
-  <si>
-    <t>Execution time</t>
   </si>
   <si>
     <t>Average</t>
@@ -37,6 +35,18 @@
   </si>
   <si>
     <t>Safari (Nitro)</t>
+  </si>
+  <si>
+    <t>Opera Mobile (Carakan)</t>
+  </si>
+  <si>
+    <t>Execution time (ms)</t>
+  </si>
+  <si>
+    <t>Android 2.3.3 (V8)</t>
+  </si>
+  <si>
+    <t>Firefox for Android (IonMonkey)</t>
   </si>
 </sst>
 </file>
@@ -118,7 +128,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -128,6 +138,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -139,6 +150,358 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'JS performance'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Chrome (V8)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'JS performance'!$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>23.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'JS performance'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox (IonMonkey)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'JS performance'!$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'JS performance'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Safari (Nitro)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'JS performance'!$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'JS performance'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Opera Mobile (Carakan)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'JS performance'!$E$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>146.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'JS performance'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Android 2.3.3 (V8)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'JS performance'!$F$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>164.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'JS performance'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Firefox for Android (IonMonkey)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'JS performance'!$G$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>166.425</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="318926040"/>
+        <c:axId val="318993176"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="318926040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="318993176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="318993176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="318926040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -463,37 +826,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>26</v>
@@ -504,8 +879,17 @@
       <c r="D2">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>355</v>
+      </c>
+      <c r="F2">
+        <v>151</v>
+      </c>
+      <c r="G2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="B3">
         <v>19</v>
       </c>
@@ -515,8 +899,17 @@
       <c r="D3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>265</v>
+      </c>
+      <c r="F3">
+        <v>171</v>
+      </c>
+      <c r="G3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="B4">
         <v>19</v>
       </c>
@@ -526,8 +919,17 @@
       <c r="D4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>125</v>
+      </c>
+      <c r="F4">
+        <v>112</v>
+      </c>
+      <c r="G4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="B5">
         <v>22</v>
       </c>
@@ -537,8 +939,17 @@
       <c r="D5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>39</v>
+      </c>
+      <c r="F5">
+        <v>276</v>
+      </c>
+      <c r="G5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="B6">
         <v>23</v>
       </c>
@@ -548,8 +959,17 @@
       <c r="D6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>63</v>
+      </c>
+      <c r="F6">
+        <v>65</v>
+      </c>
+      <c r="G6">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="B7">
         <v>29</v>
       </c>
@@ -559,8 +979,17 @@
       <c r="D7">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>70</v>
+      </c>
+      <c r="F7">
+        <v>1248</v>
+      </c>
+      <c r="G7">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="B8">
         <v>32</v>
       </c>
@@ -570,8 +999,17 @@
       <c r="D8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>51</v>
+      </c>
+      <c r="F8">
+        <v>96</v>
+      </c>
+      <c r="G8">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="B9">
         <v>19</v>
       </c>
@@ -581,8 +1019,17 @@
       <c r="D9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>52</v>
+      </c>
+      <c r="F9">
+        <v>58</v>
+      </c>
+      <c r="G9">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="B10">
         <v>23</v>
       </c>
@@ -592,8 +1039,17 @@
       <c r="D10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>55</v>
+      </c>
+      <c r="F10">
+        <v>49</v>
+      </c>
+      <c r="G10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="B11">
         <v>18</v>
       </c>
@@ -603,8 +1059,17 @@
       <c r="D11">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>40</v>
+      </c>
+      <c r="F11">
+        <v>354</v>
+      </c>
+      <c r="G11">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="B12">
         <v>17</v>
       </c>
@@ -614,8 +1079,17 @@
       <c r="D12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>98</v>
+      </c>
+      <c r="F12">
+        <v>127</v>
+      </c>
+      <c r="G12">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="B13">
         <v>35</v>
       </c>
@@ -625,8 +1099,17 @@
       <c r="D13">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>46</v>
+      </c>
+      <c r="F13">
+        <v>96</v>
+      </c>
+      <c r="G13">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="B14">
         <v>20</v>
       </c>
@@ -636,8 +1119,17 @@
       <c r="D14">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>97</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="B15">
         <v>29</v>
       </c>
@@ -647,8 +1139,17 @@
       <c r="D15">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>232</v>
+      </c>
+      <c r="F15">
+        <v>84</v>
+      </c>
+      <c r="G15">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="B16">
         <v>18</v>
       </c>
@@ -658,8 +1159,17 @@
       <c r="D16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="2:4">
+      <c r="E16">
+        <v>143</v>
+      </c>
+      <c r="F16">
+        <v>414</v>
+      </c>
+      <c r="G16">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
       <c r="B17">
         <v>42</v>
       </c>
@@ -669,8 +1179,17 @@
       <c r="D17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="2:4">
+      <c r="E17">
+        <v>160</v>
+      </c>
+      <c r="F17">
+        <v>447</v>
+      </c>
+      <c r="G17">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
       <c r="B18">
         <v>24</v>
       </c>
@@ -680,8 +1199,17 @@
       <c r="D18">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="2:4">
+      <c r="E18">
+        <v>44</v>
+      </c>
+      <c r="F18">
+        <v>79</v>
+      </c>
+      <c r="G18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
       <c r="B19">
         <v>21</v>
       </c>
@@ -691,8 +1219,17 @@
       <c r="D19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="2:4">
+      <c r="E19">
+        <v>37</v>
+      </c>
+      <c r="F19">
+        <v>238</v>
+      </c>
+      <c r="G19">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
       <c r="B20">
         <v>28</v>
       </c>
@@ -702,8 +1239,17 @@
       <c r="D20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="2:4">
+      <c r="E20">
+        <v>48</v>
+      </c>
+      <c r="F20">
+        <v>222</v>
+      </c>
+      <c r="G20">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
       <c r="B21">
         <v>21</v>
       </c>
@@ -713,8 +1259,17 @@
       <c r="D21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="2:4">
+      <c r="E21">
+        <v>38</v>
+      </c>
+      <c r="F21">
+        <v>95</v>
+      </c>
+      <c r="G21">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
       <c r="B22">
         <v>25</v>
       </c>
@@ -724,8 +1279,17 @@
       <c r="D22">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="2:4">
+      <c r="E22">
+        <v>48</v>
+      </c>
+      <c r="F22">
+        <v>42</v>
+      </c>
+      <c r="G22">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
       <c r="B23">
         <v>20</v>
       </c>
@@ -735,8 +1299,17 @@
       <c r="D23">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="2:4">
+      <c r="E23">
+        <v>42</v>
+      </c>
+      <c r="F23">
+        <v>53</v>
+      </c>
+      <c r="G23">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
       <c r="B24">
         <v>19</v>
       </c>
@@ -746,8 +1319,17 @@
       <c r="D24">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="2:4">
+      <c r="E24">
+        <v>44</v>
+      </c>
+      <c r="F24">
+        <v>59</v>
+      </c>
+      <c r="G24">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
       <c r="B25">
         <v>20</v>
       </c>
@@ -757,8 +1339,17 @@
       <c r="D25">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="2:4">
+      <c r="E25">
+        <v>44</v>
+      </c>
+      <c r="F25">
+        <v>105</v>
+      </c>
+      <c r="G25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
       <c r="B26">
         <v>19</v>
       </c>
@@ -768,8 +1359,17 @@
       <c r="D26">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="2:4">
+      <c r="E26">
+        <v>51</v>
+      </c>
+      <c r="F26">
+        <v>111</v>
+      </c>
+      <c r="G26">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
       <c r="B27">
         <v>27</v>
       </c>
@@ -779,8 +1379,17 @@
       <c r="D27">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="2:4">
+      <c r="E27">
+        <v>246</v>
+      </c>
+      <c r="F27">
+        <v>96</v>
+      </c>
+      <c r="G27">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
       <c r="B28">
         <v>24</v>
       </c>
@@ -790,8 +1399,17 @@
       <c r="D28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="2:4">
+      <c r="E28">
+        <v>104</v>
+      </c>
+      <c r="F28">
+        <v>55</v>
+      </c>
+      <c r="G28">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
       <c r="B29">
         <v>17</v>
       </c>
@@ -801,8 +1419,17 @@
       <c r="D29">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="2:4">
+      <c r="E29">
+        <v>215</v>
+      </c>
+      <c r="F29">
+        <v>243</v>
+      </c>
+      <c r="G29">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
       <c r="B30">
         <v>21</v>
       </c>
@@ -812,8 +1439,17 @@
       <c r="D30">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="2:4">
+      <c r="E30">
+        <v>215</v>
+      </c>
+      <c r="F30">
+        <v>48</v>
+      </c>
+      <c r="G30">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
       <c r="B31">
         <v>30</v>
       </c>
@@ -823,8 +1459,17 @@
       <c r="D31">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="2:4">
+      <c r="E31">
+        <v>233</v>
+      </c>
+      <c r="F31">
+        <v>152</v>
+      </c>
+      <c r="G31">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
       <c r="B32">
         <v>27</v>
       </c>
@@ -834,8 +1479,17 @@
       <c r="D32">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <v>245</v>
+      </c>
+      <c r="F32">
+        <v>81</v>
+      </c>
+      <c r="G32">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="B33">
         <v>19</v>
       </c>
@@ -845,8 +1499,17 @@
       <c r="D33">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33">
+        <v>267</v>
+      </c>
+      <c r="F33">
+        <v>85</v>
+      </c>
+      <c r="G33">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="B34">
         <v>37</v>
       </c>
@@ -856,8 +1519,17 @@
       <c r="D34">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34">
+        <v>388</v>
+      </c>
+      <c r="F34">
+        <v>129</v>
+      </c>
+      <c r="G34">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="B35">
         <v>18</v>
       </c>
@@ -867,8 +1539,17 @@
       <c r="D35">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <v>603</v>
+      </c>
+      <c r="F35">
+        <v>71</v>
+      </c>
+      <c r="G35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="B36">
         <v>33</v>
       </c>
@@ -878,8 +1559,17 @@
       <c r="D36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36">
+        <v>123</v>
+      </c>
+      <c r="F36">
+        <v>71</v>
+      </c>
+      <c r="G36">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="B37">
         <v>21</v>
       </c>
@@ -889,8 +1579,17 @@
       <c r="D37">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <v>98</v>
+      </c>
+      <c r="F37">
+        <v>53</v>
+      </c>
+      <c r="G37">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="B38">
         <v>20</v>
       </c>
@@ -900,8 +1599,17 @@
       <c r="D38">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>93</v>
+      </c>
+      <c r="F38">
+        <v>44</v>
+      </c>
+      <c r="G38">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="B39">
         <v>17</v>
       </c>
@@ -911,8 +1619,17 @@
       <c r="D39">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>211</v>
+      </c>
+      <c r="F39">
+        <v>416</v>
+      </c>
+      <c r="G39">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="B40">
         <v>19</v>
       </c>
@@ -922,8 +1639,17 @@
       <c r="D40">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <v>120</v>
+      </c>
+      <c r="F40">
+        <v>84</v>
+      </c>
+      <c r="G40">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="B41">
         <v>28</v>
       </c>
@@ -933,10 +1659,19 @@
       <c r="D41">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41">
+        <v>424</v>
+      </c>
+      <c r="F41">
+        <v>100</v>
+      </c>
+      <c r="G41">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B42" s="4">
         <f>AVERAGE(B2:B41)</f>
@@ -950,10 +1685,40 @@
         <f>AVERAGE(D2:D41)</f>
         <v>7.875</v>
       </c>
+      <c r="E42" s="4">
+        <f>AVERAGE(E2:E41)</f>
+        <v>146.80000000000001</v>
+      </c>
+      <c r="F42" s="4">
+        <f>AVERAGE(F2:F41)</f>
+        <v>164.5</v>
+      </c>
+      <c r="G42" s="4">
+        <f>AVERAGE(G2:G41)</f>
+        <v>166.42500000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Finished backend and round-trip testing. Added sections for these to chapter 4.
</commit_message>
<xml_diff>
--- a/Test data.xlsx
+++ b/Test data.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8460" windowHeight="17480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="JS performance" sheetId="1" r:id="rId1"/>
-    <sheet name="Server side response time" sheetId="2" r:id="rId2"/>
+    <sheet name="Request round-trip time" sheetId="2" r:id="rId2"/>
+    <sheet name="Backend processing time" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Browser</t>
   </si>
@@ -47,6 +48,30 @@
   </si>
   <si>
     <t>Firefox for Android (IonMonkey)</t>
+  </si>
+  <si>
+    <t>Without plugin</t>
+  </si>
+  <si>
+    <t>Interceptor redirect</t>
+  </si>
+  <si>
+    <t>Page request</t>
+  </si>
+  <si>
+    <t>Total-time</t>
+  </si>
+  <si>
+    <t>Processing-time</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>getUAFamily time</t>
   </si>
 </sst>
 </file>
@@ -121,8 +146,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -132,19 +163,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -165,7 +202,31 @@
       <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average execution time of Detector</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> JS (ms)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -404,21 +465,20 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="318926040"/>
-        <c:axId val="318993176"/>
+        <c:axId val="310899352"/>
+        <c:axId val="345501976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="318926040"/>
+        <c:axId val="310899352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318993176"/>
+        <c:crossAx val="345501976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -426,7 +486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="318993176"/>
+        <c:axId val="345501976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -444,10 +504,501 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318926040"/>
+        <c:crossAx val="310899352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> request round-trip time (ms)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Request round-trip time'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Interceptor redirect</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Request round-trip time'!$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Request round-trip time'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Page request</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Request round-trip time'!$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>828.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Request round-trip time'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Request round-trip time'!$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>849.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Request round-trip time'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Without plugin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Request round-trip time'!$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>469.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="329347160"/>
+        <c:axId val="329349832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="329347160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="329349832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="329349832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="329347160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average backend processing time (ms)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Backend processing time'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total-time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Backend processing time'!$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>646.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Backend processing time'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Processing-time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Backend processing time'!$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>254.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Backend processing time'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>getUAFamily time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Backend processing time'!$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="327942696"/>
+        <c:axId val="327945576"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="327942696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="327945576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="327945576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="327942696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -479,14 +1030,84 @@
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>208650</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>88450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>170550</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>12250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>75300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>24950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -824,12 +1445,566 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="1F497D"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="EEECE1"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4F81BD"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="C0504D"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="9BBB59"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="8064A2"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4BACC6"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="F79646"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0000FF"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="800080"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="100000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride2.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="1F497D"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="EEECE1"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4F81BD"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="C0504D"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="9BBB59"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="8064A2"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4BACC6"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="F79646"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0000FF"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="800080"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="100000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -847,13 +2022,13 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="7" t="s">
@@ -1073,7 +2248,7 @@
       <c r="B12">
         <v>17</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>10</v>
       </c>
       <c r="D12">
@@ -1670,30 +2845,30 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="3">
         <f>AVERAGE(B2:B41)</f>
         <v>23.65</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="3">
         <f>AVERAGE(C2:C41)</f>
         <v>10.125</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="3">
         <f>AVERAGE(D2:D41)</f>
         <v>7.875</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="3">
         <f>AVERAGE(E2:E41)</f>
         <v>146.80000000000001</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F42" s="3">
         <f>AVERAGE(F2:F41)</f>
         <v>164.5</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="3">
         <f>AVERAGE(G2:G41)</f>
         <v>166.42500000000001</v>
       </c>
@@ -1712,13 +2887,642 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>2026</v>
+      </c>
+      <c r="D2">
+        <f>SUM(B2:C2)</f>
+        <v>2061</v>
+      </c>
+      <c r="E2">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>1205</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D21" si="0">SUM(B3:C3)</f>
+        <v>1216</v>
+      </c>
+      <c r="E3">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>1002</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1014</v>
+      </c>
+      <c r="E4">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>1091</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1102</v>
+      </c>
+      <c r="E5">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>1020</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1034</v>
+      </c>
+      <c r="E6">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>879</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>889</v>
+      </c>
+      <c r="E7">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>992</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1003</v>
+      </c>
+      <c r="E8">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>645</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>656</v>
+      </c>
+      <c r="E9">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>636</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>646</v>
+      </c>
+      <c r="E10">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11">
+        <v>171</v>
+      </c>
+      <c r="C11">
+        <v>620</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>791</v>
+      </c>
+      <c r="E11">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>768</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>780</v>
+      </c>
+      <c r="E12">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>736</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>744</v>
+      </c>
+      <c r="E13">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>635</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>653</v>
+      </c>
+      <c r="E14">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>554</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>565</v>
+      </c>
+      <c r="E15">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>1165</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1183</v>
+      </c>
+      <c r="E16">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>552</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>562</v>
+      </c>
+      <c r="E17">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>528</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>540</v>
+      </c>
+      <c r="E18">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>484</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>495</v>
+      </c>
+      <c r="E19">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>503</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>511</v>
+      </c>
+      <c r="E20">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>538</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>548</v>
+      </c>
+      <c r="E21">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" ref="B22:D22" si="1">AVERAGE(B2:B21)</f>
+        <v>20.7</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="1"/>
+        <v>828.95</v>
+      </c>
+      <c r="D22" s="3">
+        <f>AVERAGE(D2:D21)</f>
+        <v>849.65</v>
+      </c>
+      <c r="E22" s="3">
+        <f>AVERAGE(E2:E21)</f>
+        <v>469.7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>2046</v>
+      </c>
+      <c r="C2">
+        <v>866</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3">
+        <v>1012</v>
+      </c>
+      <c r="C3">
+        <v>366</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4">
+        <v>733</v>
+      </c>
+      <c r="C4">
+        <v>305</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5">
+        <v>667</v>
+      </c>
+      <c r="C5">
+        <v>236</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6">
+        <v>953</v>
+      </c>
+      <c r="C6">
+        <v>261</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7">
+        <v>687</v>
+      </c>
+      <c r="C7">
+        <v>247</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8">
+        <v>525</v>
+      </c>
+      <c r="C8">
+        <v>225</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9">
+        <v>725</v>
+      </c>
+      <c r="C9">
+        <v>339</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10">
+        <v>494</v>
+      </c>
+      <c r="C10">
+        <v>180</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11">
+        <v>472</v>
+      </c>
+      <c r="C11">
+        <v>190</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12">
+        <v>465</v>
+      </c>
+      <c r="C12">
+        <v>177</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13">
+        <v>480</v>
+      </c>
+      <c r="C13">
+        <v>200</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14">
+        <v>647</v>
+      </c>
+      <c r="C14">
+        <v>256</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15">
+        <v>436</v>
+      </c>
+      <c r="C15">
+        <v>179</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16">
+        <v>476</v>
+      </c>
+      <c r="C16">
+        <v>205</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="B17">
+        <v>438</v>
+      </c>
+      <c r="C17">
+        <v>168</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="B18">
+        <v>428</v>
+      </c>
+      <c r="C18">
+        <v>180</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="B19">
+        <v>451</v>
+      </c>
+      <c r="C19">
+        <v>180</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="B20">
+        <v>383</v>
+      </c>
+      <c r="C20">
+        <v>155</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="B21">
+        <v>413</v>
+      </c>
+      <c r="C21">
+        <v>176</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" ref="B22:D22" si="0">AVERAGE(B2:B21)</f>
+        <v>646.54999999999995</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>254.55</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Changed line height, added more to chapter 4. Edited chapter 3. Started adding citations.
</commit_message>
<xml_diff>
--- a/Test data.xlsx
+++ b/Test data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8460" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="17480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="JS performance" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Browser</t>
   </si>
@@ -65,13 +65,16 @@
     <t>Processing-time</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Time (ms)</t>
   </si>
   <si>
     <t>getUAFamily time</t>
+  </si>
+  <si>
+    <t>With plugin, no redirect</t>
+  </si>
+  <si>
+    <t>Total w/ redirect</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -145,8 +148,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -158,8 +192,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -168,20 +206,27 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -542,6 +587,7 @@
       <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -554,11 +600,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Average</a:t>
+              <a:t>Average request</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> request round-trip time (ms)</a:t>
+              <a:t> round-trip time (ms)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -657,7 +703,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total</c:v>
+                  <c:v>Total w/ redirect</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -694,7 +740,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Without plugin</c:v>
+                  <c:v>With plugin, no redirect</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -716,6 +762,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
+                  <c:v>453.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Request round-trip time'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Without plugin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Request round-trip time'!$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>469.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -731,11 +814,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="329347160"/>
-        <c:axId val="329349832"/>
+        <c:axId val="345215880"/>
+        <c:axId val="345241832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="329347160"/>
+        <c:axId val="345215880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -744,7 +827,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="329349832"/>
+        <c:crossAx val="345241832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -752,7 +835,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="329349832"/>
+        <c:axId val="345241832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -773,7 +856,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="329347160"/>
+        <c:crossAx val="345215880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1025,15 +1108,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>208650</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>88450</xdr:rowOff>
+      <xdr:colOff>94350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>177350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1059,20 +1142,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>170550</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>12250</xdr:rowOff>
+      <xdr:colOff>691250</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>190050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1095,15 +1178,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>75300</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>24950</xdr:rowOff>
+      <xdr:colOff>151500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>101150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1999,12 +2082,289 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride3.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="1F497D"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="EEECE1"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4F81BD"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="C0504D"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="9BBB59"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="8064A2"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4BACC6"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="F79646"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0000FF"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="800080"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="100000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2031,13 +2391,13 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2890,7 +3250,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2899,8 +3259,9 @@
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2911,17 +3272,19 @@
       <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>35</v>
@@ -2929,11 +3292,14 @@
       <c r="C2">
         <v>2026</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="9">
         <f>SUM(B2:C2)</f>
         <v>2061</v>
       </c>
       <c r="E2">
+        <v>604</v>
+      </c>
+      <c r="F2">
         <v>888</v>
       </c>
     </row>
@@ -2944,11 +3310,14 @@
       <c r="C3">
         <v>1205</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="9">
         <f t="shared" ref="D3:D21" si="0">SUM(B3:C3)</f>
         <v>1216</v>
       </c>
       <c r="E3">
+        <v>504</v>
+      </c>
+      <c r="F3">
         <v>614</v>
       </c>
     </row>
@@ -2959,11 +3328,14 @@
       <c r="C4">
         <v>1002</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="9">
         <f t="shared" si="0"/>
         <v>1014</v>
       </c>
       <c r="E4">
+        <v>457</v>
+      </c>
+      <c r="F4">
         <v>463</v>
       </c>
     </row>
@@ -2974,11 +3346,14 @@
       <c r="C5">
         <v>1091</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="9">
         <f t="shared" si="0"/>
         <v>1102</v>
       </c>
       <c r="E5">
+        <v>501</v>
+      </c>
+      <c r="F5">
         <v>437</v>
       </c>
     </row>
@@ -2989,11 +3364,14 @@
       <c r="C6">
         <v>1020</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="9">
         <f t="shared" si="0"/>
         <v>1034</v>
       </c>
       <c r="E6">
+        <v>421</v>
+      </c>
+      <c r="F6">
         <v>563</v>
       </c>
     </row>
@@ -3004,11 +3382,14 @@
       <c r="C7">
         <v>879</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="9">
         <f t="shared" si="0"/>
         <v>889</v>
       </c>
       <c r="E7">
+        <v>441</v>
+      </c>
+      <c r="F7">
         <v>503</v>
       </c>
     </row>
@@ -3019,11 +3400,14 @@
       <c r="C8">
         <v>992</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="9">
         <f t="shared" si="0"/>
         <v>1003</v>
       </c>
       <c r="E8">
+        <v>414</v>
+      </c>
+      <c r="F8">
         <v>516</v>
       </c>
     </row>
@@ -3034,11 +3418,14 @@
       <c r="C9">
         <v>645</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="9">
         <f t="shared" si="0"/>
         <v>656</v>
       </c>
       <c r="E9">
+        <v>466</v>
+      </c>
+      <c r="F9">
         <v>432</v>
       </c>
     </row>
@@ -3049,11 +3436,14 @@
       <c r="C10">
         <v>636</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="9">
         <f t="shared" si="0"/>
         <v>646</v>
       </c>
       <c r="E10">
+        <v>455</v>
+      </c>
+      <c r="F10">
         <v>358</v>
       </c>
     </row>
@@ -3064,11 +3454,14 @@
       <c r="C11">
         <v>620</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="9">
         <f t="shared" si="0"/>
         <v>791</v>
       </c>
       <c r="E11">
+        <v>420</v>
+      </c>
+      <c r="F11">
         <v>484</v>
       </c>
     </row>
@@ -3079,11 +3472,14 @@
       <c r="C12">
         <v>768</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="9">
         <f t="shared" si="0"/>
         <v>780</v>
       </c>
       <c r="E12">
+        <v>439</v>
+      </c>
+      <c r="F12">
         <v>454</v>
       </c>
     </row>
@@ -3094,11 +3490,14 @@
       <c r="C13">
         <v>736</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="9">
         <f t="shared" si="0"/>
         <v>744</v>
       </c>
       <c r="E13">
+        <v>424</v>
+      </c>
+      <c r="F13">
         <v>438</v>
       </c>
     </row>
@@ -3109,11 +3508,14 @@
       <c r="C14">
         <v>635</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="9">
         <f t="shared" si="0"/>
         <v>653</v>
       </c>
       <c r="E14">
+        <v>598</v>
+      </c>
+      <c r="F14">
         <v>428</v>
       </c>
     </row>
@@ -3124,11 +3526,14 @@
       <c r="C15">
         <v>554</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="9">
         <f t="shared" si="0"/>
         <v>565</v>
       </c>
       <c r="E15">
+        <v>403</v>
+      </c>
+      <c r="F15">
         <v>399</v>
       </c>
     </row>
@@ -3139,90 +3544,108 @@
       <c r="C16">
         <v>1165</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="9">
         <f t="shared" si="0"/>
         <v>1183</v>
       </c>
       <c r="E16">
+        <v>501</v>
+      </c>
+      <c r="F16">
         <v>382</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="B17">
         <v>10</v>
       </c>
       <c r="C17">
         <v>552</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="9">
         <f t="shared" si="0"/>
         <v>562</v>
       </c>
       <c r="E17">
+        <v>422</v>
+      </c>
+      <c r="F17">
         <v>421</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="B18">
         <v>12</v>
       </c>
       <c r="C18">
         <v>528</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="9">
         <f t="shared" si="0"/>
         <v>540</v>
       </c>
       <c r="E18">
+        <v>409</v>
+      </c>
+      <c r="F18">
         <v>421</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="B19">
         <v>11</v>
       </c>
       <c r="C19">
         <v>484</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="9">
         <f t="shared" si="0"/>
         <v>495</v>
       </c>
       <c r="E19">
+        <v>369</v>
+      </c>
+      <c r="F19">
         <v>348</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="B20">
         <v>8</v>
       </c>
       <c r="C20">
         <v>503</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="9">
         <f t="shared" si="0"/>
         <v>511</v>
       </c>
       <c r="E20">
+        <v>386</v>
+      </c>
+      <c r="F20">
         <v>384</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="B21">
         <v>10</v>
       </c>
       <c r="C21">
         <v>538</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="9">
         <f t="shared" si="0"/>
         <v>548</v>
       </c>
       <c r="E21">
+        <v>437</v>
+      </c>
+      <c r="F21">
         <v>461</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -3234,17 +3657,22 @@
         <f t="shared" si="1"/>
         <v>828.95</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="10">
         <f>AVERAGE(D2:D21)</f>
         <v>849.65</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="7">
         <f>AVERAGE(E2:E21)</f>
+        <v>453.55</v>
+      </c>
+      <c r="F22" s="3">
+        <f>AVERAGE(F2:F21)</f>
         <v>469.7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3277,12 +3705,12 @@
         <v>13</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>2046</v>

</xml_diff>